<commit_message>
Replacing age variable numeric to grouped in multivariate analysis
</commit_message>
<xml_diff>
--- a/Output/reliability_quality_of_life.xlsx
+++ b/Output/reliability_quality_of_life.xlsx
@@ -613,7 +613,7 @@
         <v>0.7884288185556082</v>
       </c>
       <c r="D4">
-        <v>0.8065619354999315</v>
+        <v>0.8065619354999314</v>
       </c>
       <c r="E4">
         <v>0.2928165207030181</v>
@@ -644,7 +644,7 @@
         <v>0.8030555782218118</v>
       </c>
       <c r="D5">
-        <v>0.8209411566149183</v>
+        <v>0.8209411566149184</v>
       </c>
       <c r="E5">
         <v>0.3117989953771809</v>
@@ -675,7 +675,7 @@
         <v>0.8018533182932462</v>
       </c>
       <c r="D6">
-        <v>0.8205745423903787</v>
+        <v>0.8205745423903789</v>
       </c>
       <c r="E6">
         <v>0.3101738945833059</v>
@@ -737,7 +737,7 @@
         <v>0.826864728544615</v>
       </c>
       <c r="D8">
-        <v>0.8367452225507059</v>
+        <v>0.8367452225507058</v>
       </c>
       <c r="E8">
         <v>0.3466818621074966</v>
@@ -768,7 +768,7 @@
         <v>0.811923348065488</v>
       </c>
       <c r="D9">
-        <v>0.8263291680442781</v>
+        <v>0.826329168044278</v>
       </c>
       <c r="E9">
         <v>0.3241711506785097</v>
@@ -830,7 +830,7 @@
         <v>0.8094055345752785</v>
       </c>
       <c r="D11">
-        <v>0.830416294292195</v>
+        <v>0.8304162942921951</v>
       </c>
       <c r="E11">
         <v>0.3205876620356739</v>
@@ -919,7 +919,7 @@
         <v>0.5966459158117254</v>
       </c>
       <c r="E2">
-        <v>0.5438101930836244</v>
+        <v>0.5438101930836243</v>
       </c>
       <c r="F2">
         <v>0.4893561565805778</v>
@@ -975,7 +975,7 @@
         <v>0.8262743170159947</v>
       </c>
       <c r="E4">
-        <v>0.8341952027652852</v>
+        <v>0.8341952027652854</v>
       </c>
       <c r="F4">
         <v>0.7701337375955195</v>
@@ -1003,7 +1003,7 @@
         <v>0.7174931413078909</v>
       </c>
       <c r="E5">
-        <v>0.6938532256908548</v>
+        <v>0.6938532256908551</v>
       </c>
       <c r="F5">
         <v>0.6320094231477831</v>
@@ -1143,7 +1143,7 @@
         <v>0.6653313937583882</v>
       </c>
       <c r="E10">
-        <v>0.614069760617324</v>
+        <v>0.6140697606173241</v>
       </c>
       <c r="F10">
         <v>0.5655017351225673</v>
@@ -1171,7 +1171,7 @@
         <v>0.6671287126215318</v>
       </c>
       <c r="E11">
-        <v>0.6152308717985094</v>
+        <v>0.6152308717985093</v>
       </c>
       <c r="F11">
         <v>0.5640592637101439</v>

</xml_diff>